<commit_message>
feat: Add Docker and Kubernetes CI/CD pipeline
</commit_message>
<xml_diff>
--- a/data/namasthe_hounslow_menu.xlsx
+++ b/data/namasthe_hounslow_menu.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="174">
   <si>
     <t>Price</t>
   </si>
@@ -541,144 +541,6 @@
   </si>
   <si>
     <t>WINES (125 ml)</t>
-  </si>
-  <si>
-    <t>Emoji</t>
-  </si>
-  <si>
-    <t>🍚</t>
-  </si>
-  <si>
-    <t>✨</t>
-  </si>
-  <si>
-    <t>🥣</t>
-  </si>
-  <si>
-    <t>🍩</t>
-  </si>
-  <si>
-    <t>🍽️</t>
-  </si>
-  <si>
-    <t>🥞</t>
-  </si>
-  <si>
-    <t>🧅</t>
-  </si>
-  <si>
-    <t>🥔</t>
-  </si>
-  <si>
-    <t>🌶️</t>
-  </si>
-  <si>
-    <t>⭐</t>
-  </si>
-  <si>
-    <t>🧀</t>
-  </si>
-  <si>
-    <t>🥚</t>
-  </si>
-  <si>
-    <t>🥕</t>
-  </si>
-  <si>
-    <t>🍛</t>
-  </si>
-  <si>
-    <t>🍮</t>
-  </si>
-  <si>
-    <t>🍗</t>
-  </si>
-  <si>
-    <t>🍖</t>
-  </si>
-  <si>
-    <t>🌿</t>
-  </si>
-  <si>
-    <t>🍞</t>
-  </si>
-  <si>
-    <t>🥟</t>
-  </si>
-  <si>
-    <t>🫔</t>
-  </si>
-  <si>
-    <t>🍘</t>
-  </si>
-  <si>
-    <t>🥦</t>
-  </si>
-  <si>
-    <t>🥜</t>
-  </si>
-  <si>
-    <t>🍟</t>
-  </si>
-  <si>
-    <t>🍤</t>
-  </si>
-  <si>
-    <t>🍢</t>
-  </si>
-  <si>
-    <t>🍅</t>
-  </si>
-  <si>
-    <t>🍆</t>
-  </si>
-  <si>
-    <t>spinach</t>
-  </si>
-  <si>
-    <t>🔥</t>
-  </si>
-  <si>
-    <t>🍜</t>
-  </si>
-  <si>
-    <t>🐟</t>
-  </si>
-  <si>
-    <t>🧈</t>
-  </si>
-  <si>
-    <t>🍸</t>
-  </si>
-  <si>
-    <t>🥃</t>
-  </si>
-  <si>
-    <t>🍹</t>
-  </si>
-  <si>
-    <t>🍉</t>
-  </si>
-  <si>
-    <t>💣</t>
-  </si>
-  <si>
-    <t>🍷</t>
-  </si>
-  <si>
-    <t>🌵</t>
-  </si>
-  <si>
-    <t>🧉</t>
-  </si>
-  <si>
-    <t>🥥</t>
-  </si>
-  <si>
-    <t>🍺</t>
-  </si>
-  <si>
-    <t>🍾</t>
   </si>
 </sst>
 </file>
@@ -742,12 +604,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1055,32 +916,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D157"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="8.7265625" style="2"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>168</v>
       </c>
@@ -1090,11 +945,8 @@
       <c r="C2" s="1">
         <v>4.99</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>168</v>
       </c>
@@ -1104,11 +956,8 @@
       <c r="C3" s="1">
         <v>5.99</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>168</v>
       </c>
@@ -1118,11 +967,8 @@
       <c r="C4" s="1">
         <v>5.5</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>168</v>
       </c>
@@ -1132,11 +978,8 @@
       <c r="C5" s="1">
         <v>5.99</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>168</v>
       </c>
@@ -1146,11 +989,8 @@
       <c r="C6" s="1">
         <v>6.99</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>168</v>
       </c>
@@ -1160,11 +1000,8 @@
       <c r="C7" s="1">
         <v>7.99</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>168</v>
       </c>
@@ -1174,11 +1011,8 @@
       <c r="C8" s="1">
         <v>4.5</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>168</v>
       </c>
@@ -1188,11 +1022,8 @@
       <c r="C9" s="1">
         <v>4.99</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>168</v>
       </c>
@@ -1202,11 +1033,8 @@
       <c r="C10" s="1">
         <v>6.99</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>168</v>
       </c>
@@ -1216,11 +1044,8 @@
       <c r="C11" s="1">
         <v>6.99</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
@@ -1230,11 +1055,8 @@
       <c r="C12" s="1">
         <v>6.99</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
@@ -1244,11 +1066,8 @@
       <c r="C13" s="1">
         <v>5.99</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>168</v>
       </c>
@@ -1258,11 +1077,8 @@
       <c r="C14" s="1">
         <v>7.99</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>168</v>
       </c>
@@ -1272,11 +1088,8 @@
       <c r="C15" s="1">
         <v>7.99</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>168</v>
       </c>
@@ -1286,11 +1099,8 @@
       <c r="C16" s="1">
         <v>8.99</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>168</v>
       </c>
@@ -1300,11 +1110,8 @@
       <c r="C17" s="1">
         <v>7.99</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>168</v>
       </c>
@@ -1314,11 +1121,8 @@
       <c r="C18" s="1">
         <v>5.99</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>168</v>
       </c>
@@ -1328,11 +1132,8 @@
       <c r="C19" s="1">
         <v>6.99</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>168</v>
       </c>
@@ -1342,11 +1143,8 @@
       <c r="C20" s="1">
         <v>5.99</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -1356,11 +1154,8 @@
       <c r="C21" s="1">
         <v>5.99</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>168</v>
       </c>
@@ -1370,11 +1165,8 @@
       <c r="C22" s="1">
         <v>7.99</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>168</v>
       </c>
@@ -1384,11 +1176,8 @@
       <c r="C23" s="1">
         <v>6.99</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>168</v>
       </c>
@@ -1398,11 +1187,8 @@
       <c r="C24" s="1">
         <v>8.99</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>168</v>
       </c>
@@ -1412,11 +1198,8 @@
       <c r="C25" s="1">
         <v>9.99</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>168</v>
       </c>
@@ -1426,11 +1209,8 @@
       <c r="C26" s="1">
         <v>9.99</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>168</v>
       </c>
@@ -1440,11 +1220,8 @@
       <c r="C27" s="1">
         <v>6.99</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>168</v>
       </c>
@@ -1454,11 +1231,8 @@
       <c r="C28" s="1">
         <v>5.5</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>168</v>
       </c>
@@ -1468,11 +1242,8 @@
       <c r="C29" s="1">
         <v>6.99</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>168</v>
       </c>
@@ -1482,11 +1253,8 @@
       <c r="C30" s="1">
         <v>4.99</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>168</v>
       </c>
@@ -1496,11 +1264,8 @@
       <c r="C31" s="1">
         <v>6.99</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>168</v>
       </c>
@@ -1510,11 +1275,8 @@
       <c r="C32" s="1">
         <v>2</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>169</v>
       </c>
@@ -1524,11 +1286,8 @@
       <c r="C33" s="1">
         <v>3.99</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>169</v>
       </c>
@@ -1538,11 +1297,8 @@
       <c r="C34" s="1">
         <v>3.99</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>169</v>
       </c>
@@ -1552,11 +1308,8 @@
       <c r="C35" s="1">
         <v>4.99</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>169</v>
       </c>
@@ -1566,11 +1319,8 @@
       <c r="C36" s="1">
         <v>4.99</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>169</v>
       </c>
@@ -1580,11 +1330,8 @@
       <c r="C37" s="1">
         <v>6.99</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>169</v>
       </c>
@@ -1594,11 +1341,8 @@
       <c r="C38" s="1">
         <v>4.99</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>169</v>
       </c>
@@ -1608,11 +1352,8 @@
       <c r="C39" s="1">
         <v>3.99</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>169</v>
       </c>
@@ -1622,11 +1363,8 @@
       <c r="C40" s="1">
         <v>3.99</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>169</v>
       </c>
@@ -1636,11 +1374,8 @@
       <c r="C41" s="1">
         <v>2.99</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>169</v>
       </c>
@@ -1650,11 +1385,8 @@
       <c r="C42" s="1">
         <v>1.25</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>169</v>
       </c>
@@ -1664,11 +1396,8 @@
       <c r="C43" s="1">
         <v>1.5</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>169</v>
       </c>
@@ -1678,11 +1407,8 @@
       <c r="C44" s="1">
         <v>4.99</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>169</v>
       </c>
@@ -1692,11 +1418,8 @@
       <c r="C45" s="1">
         <v>8.99</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>169</v>
       </c>
@@ -1706,11 +1429,8 @@
       <c r="C46" s="1">
         <v>8.99</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>169</v>
       </c>
@@ -1720,11 +1440,8 @@
       <c r="C47" s="1">
         <v>8.99</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>169</v>
       </c>
@@ -1734,11 +1451,8 @@
       <c r="C48" s="1">
         <v>9.99</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>169</v>
       </c>
@@ -1748,11 +1462,8 @@
       <c r="C49" s="1">
         <v>9.99</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>169</v>
       </c>
@@ -1762,11 +1473,8 @@
       <c r="C50" s="1">
         <v>9.99</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>169</v>
       </c>
@@ -1776,11 +1484,8 @@
       <c r="C51" s="1">
         <v>8.99</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>169</v>
       </c>
@@ -1790,11 +1495,8 @@
       <c r="C52" s="1">
         <v>8.99</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>170</v>
       </c>
@@ -1804,11 +1506,8 @@
       <c r="C53" s="1">
         <v>4.99</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>170</v>
       </c>
@@ -1818,11 +1517,8 @@
       <c r="C54" s="1">
         <v>5.99</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>170</v>
       </c>
@@ -1832,11 +1528,8 @@
       <c r="C55" s="1">
         <v>6.99</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>170</v>
       </c>
@@ -1846,11 +1539,8 @@
       <c r="C56" s="1">
         <v>7.99</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>170</v>
       </c>
@@ -1860,11 +1550,8 @@
       <c r="C57" s="1">
         <v>9.99</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>170</v>
       </c>
@@ -1874,11 +1561,8 @@
       <c r="C58" s="1">
         <v>9.99</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>170</v>
       </c>
@@ -1888,11 +1572,8 @@
       <c r="C59" s="1">
         <v>7.99</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>170</v>
       </c>
@@ -1902,11 +1583,8 @@
       <c r="C60" s="1">
         <v>7.99</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>170</v>
       </c>
@@ -1916,11 +1594,8 @@
       <c r="C61" s="1">
         <v>9.99</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>170</v>
       </c>
@@ -1930,11 +1605,8 @@
       <c r="C62" s="1">
         <v>8.99</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>170</v>
       </c>
@@ -1944,11 +1616,8 @@
       <c r="C63" s="1">
         <v>8.99</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>170</v>
       </c>
@@ -1958,11 +1627,8 @@
       <c r="C64" s="1">
         <v>9.99</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>170</v>
       </c>
@@ -1972,11 +1638,8 @@
       <c r="C65" s="1">
         <v>11.99</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>171</v>
       </c>
@@ -1986,11 +1649,8 @@
       <c r="C66" s="1">
         <v>8.99</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>171</v>
       </c>
@@ -2000,11 +1660,8 @@
       <c r="C67" s="1">
         <v>9.99</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>171</v>
       </c>
@@ -2014,11 +1671,8 @@
       <c r="C68" s="1">
         <v>9.99</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>171</v>
       </c>
@@ -2028,11 +1682,8 @@
       <c r="C69" s="1">
         <v>8.99</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>172</v>
       </c>
@@ -2042,11 +1693,8 @@
       <c r="C70" s="1">
         <v>10.99</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>172</v>
       </c>
@@ -2056,11 +1704,8 @@
       <c r="C71" s="1">
         <v>12.99</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>172</v>
       </c>
@@ -2070,11 +1715,8 @@
       <c r="C72" s="1">
         <v>10.99</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>172</v>
       </c>
@@ -2084,11 +1726,8 @@
       <c r="C73" s="1">
         <v>12.99</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>153</v>
       </c>
@@ -2098,11 +1737,8 @@
       <c r="C74" s="1">
         <v>4.99</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>153</v>
       </c>
@@ -2112,11 +1748,8 @@
       <c r="C75" s="1">
         <v>7.99</v>
       </c>
-      <c r="D75" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>153</v>
       </c>
@@ -2126,11 +1759,8 @@
       <c r="C76" s="1">
         <v>10.99</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>153</v>
       </c>
@@ -2140,11 +1770,8 @@
       <c r="C77" s="1">
         <v>7.99</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>153</v>
       </c>
@@ -2154,11 +1781,8 @@
       <c r="C78" s="1">
         <v>9.99</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>153</v>
       </c>
@@ -2168,11 +1792,8 @@
       <c r="C79" s="1">
         <v>9.99</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>153</v>
       </c>
@@ -2182,11 +1803,8 @@
       <c r="C80" s="1">
         <v>11.99</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>153</v>
       </c>
@@ -2196,11 +1814,8 @@
       <c r="C81" s="1">
         <v>9.99</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -2210,11 +1825,8 @@
       <c r="C82" s="1">
         <v>1.99</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>154</v>
       </c>
@@ -2224,11 +1836,8 @@
       <c r="C83" s="1">
         <v>2.5</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>154</v>
       </c>
@@ -2238,11 +1847,8 @@
       <c r="C84" s="1">
         <v>1.75</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>155</v>
       </c>
@@ -2252,11 +1858,8 @@
       <c r="C85" s="1">
         <v>11.99</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>155</v>
       </c>
@@ -2266,11 +1869,8 @@
       <c r="C86" s="1">
         <v>9.99</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>155</v>
       </c>
@@ -2280,11 +1880,8 @@
       <c r="C87" s="1">
         <v>9.99</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>155</v>
       </c>
@@ -2294,11 +1891,8 @@
       <c r="C88" s="1">
         <v>9.99</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>155</v>
       </c>
@@ -2308,11 +1902,8 @@
       <c r="C89" s="1">
         <v>8.99</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>155</v>
       </c>
@@ -2322,11 +1913,8 @@
       <c r="C90" s="1">
         <v>6.99</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>155</v>
       </c>
@@ -2336,11 +1924,8 @@
       <c r="C91" s="1">
         <v>8.99</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>156</v>
       </c>
@@ -2350,11 +1935,8 @@
       <c r="C92" s="1">
         <v>2.95</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>156</v>
       </c>
@@ -2364,11 +1946,8 @@
       <c r="C93" s="1">
         <v>3.25</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>156</v>
       </c>
@@ -2378,11 +1957,8 @@
       <c r="C94" s="1">
         <v>2.95</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>157</v>
       </c>
@@ -2392,11 +1968,8 @@
       <c r="C95" s="1">
         <v>6.5</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>157</v>
       </c>
@@ -2406,11 +1979,8 @@
       <c r="C96" s="1">
         <v>9.5</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>157</v>
       </c>
@@ -2420,11 +1990,8 @@
       <c r="C97" s="1">
         <v>7.5</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>157</v>
       </c>
@@ -2434,11 +2001,8 @@
       <c r="C98" s="1">
         <v>9.5</v>
       </c>
-      <c r="D98" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>157</v>
       </c>
@@ -2448,11 +2012,8 @@
       <c r="C99" s="1">
         <v>6.5</v>
       </c>
-      <c r="D99" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>157</v>
       </c>
@@ -2462,11 +2023,8 @@
       <c r="C100" s="1">
         <v>8.5</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>157</v>
       </c>
@@ -2476,11 +2034,8 @@
       <c r="C101" s="1">
         <v>8.5</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>157</v>
       </c>
@@ -2490,11 +2045,8 @@
       <c r="C102" s="1">
         <v>6.5</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>157</v>
       </c>
@@ -2504,11 +2056,8 @@
       <c r="C103" s="1">
         <v>6.5</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>157</v>
       </c>
@@ -2518,11 +2067,8 @@
       <c r="C104" s="1">
         <v>8.5</v>
       </c>
-      <c r="D104" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>157</v>
       </c>
@@ -2532,11 +2078,8 @@
       <c r="C105" s="1">
         <v>8.5</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>157</v>
       </c>
@@ -2546,11 +2089,8 @@
       <c r="C106" s="1">
         <v>7.5</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>158</v>
       </c>
@@ -2560,11 +2100,8 @@
       <c r="C107" s="1">
         <v>6.5</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>158</v>
       </c>
@@ -2574,11 +2111,8 @@
       <c r="C108" s="1">
         <v>5.5</v>
       </c>
-      <c r="D108" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>158</v>
       </c>
@@ -2588,11 +2122,8 @@
       <c r="C109" s="1">
         <v>7.5</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>158</v>
       </c>
@@ -2602,11 +2133,8 @@
       <c r="C110" s="1">
         <v>6.5</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>158</v>
       </c>
@@ -2616,11 +2144,8 @@
       <c r="C111" s="1">
         <v>6</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>159</v>
       </c>
@@ -2630,11 +2155,8 @@
       <c r="C112" s="1">
         <v>4.99</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>159</v>
       </c>
@@ -2644,11 +2166,8 @@
       <c r="C113" s="1">
         <v>7.99</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>159</v>
       </c>
@@ -2658,11 +2177,8 @@
       <c r="C114" s="1">
         <v>5.99</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>159</v>
       </c>
@@ -2672,11 +2188,8 @@
       <c r="C115" s="1">
         <v>5.99</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>159</v>
       </c>
@@ -2686,11 +2199,8 @@
       <c r="C116" s="1">
         <v>7.99</v>
       </c>
-      <c r="D116" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>159</v>
       </c>
@@ -2700,11 +2210,8 @@
       <c r="C117" s="1">
         <v>4.99</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>159</v>
       </c>
@@ -2714,11 +2221,8 @@
       <c r="C118" s="1">
         <v>7.99</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>159</v>
       </c>
@@ -2728,11 +2232,8 @@
       <c r="C119" s="1">
         <v>6.99</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>159</v>
       </c>
@@ -2742,11 +2243,8 @@
       <c r="C120" s="1">
         <v>10.99</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>159</v>
       </c>
@@ -2756,11 +2254,8 @@
       <c r="C121" s="1">
         <v>9.99</v>
       </c>
-      <c r="D121" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>159</v>
       </c>
@@ -2770,11 +2265,8 @@
       <c r="C122" s="1">
         <v>13.99</v>
       </c>
-      <c r="D122" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>159</v>
       </c>
@@ -2784,11 +2276,8 @@
       <c r="C123" s="1">
         <v>7.99</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>159</v>
       </c>
@@ -2798,11 +2287,8 @@
       <c r="C124" s="1">
         <v>4.99</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>160</v>
       </c>
@@ -2812,11 +2298,8 @@
       <c r="C125" s="1">
         <v>6.99</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>160</v>
       </c>
@@ -2826,11 +2309,8 @@
       <c r="C126" s="1">
         <v>7.99</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>161</v>
       </c>
@@ -2840,11 +2320,8 @@
       <c r="C127" s="1">
         <v>6.99</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>161</v>
       </c>
@@ -2854,11 +2331,8 @@
       <c r="C128" s="1">
         <v>8.99</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>162</v>
       </c>
@@ -2868,11 +2342,8 @@
       <c r="C129" s="1">
         <v>5.99</v>
       </c>
-      <c r="D129" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>162</v>
       </c>
@@ -2882,11 +2353,8 @@
       <c r="C130" s="1">
         <v>5.99</v>
       </c>
-      <c r="D130" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>162</v>
       </c>
@@ -2896,11 +2364,8 @@
       <c r="C131" s="1">
         <v>8.99</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>163</v>
       </c>
@@ -2910,11 +2375,8 @@
       <c r="C132" s="1">
         <v>7.99</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="133" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>163</v>
       </c>
@@ -2924,11 +2386,8 @@
       <c r="C133" s="1">
         <v>8.99</v>
       </c>
-      <c r="D133" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>163</v>
       </c>
@@ -2938,11 +2397,8 @@
       <c r="C134" s="1">
         <v>10.99</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>163</v>
       </c>
@@ -2952,11 +2408,8 @@
       <c r="C135" s="1">
         <v>12.99</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>163</v>
       </c>
@@ -2966,11 +2419,8 @@
       <c r="C136" s="1">
         <v>13.99</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>164</v>
       </c>
@@ -2980,11 +2430,8 @@
       <c r="C137" s="1">
         <v>5.99</v>
       </c>
-      <c r="D137" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>164</v>
       </c>
@@ -2994,11 +2441,8 @@
       <c r="C138" s="1">
         <v>6.99</v>
       </c>
-      <c r="D138" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>164</v>
       </c>
@@ -3008,11 +2452,8 @@
       <c r="C139" s="1">
         <v>6.99</v>
       </c>
-      <c r="D139" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>164</v>
       </c>
@@ -3022,11 +2463,8 @@
       <c r="C140" s="1">
         <v>5.99</v>
       </c>
-      <c r="D140" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>164</v>
       </c>
@@ -3036,11 +2474,8 @@
       <c r="C141" s="1">
         <v>5.99</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>164</v>
       </c>
@@ -3050,11 +2485,8 @@
       <c r="C142" s="1">
         <v>6.99</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>165</v>
       </c>
@@ -3064,11 +2496,8 @@
       <c r="C143" s="1">
         <v>3.99</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>165</v>
       </c>
@@ -3078,11 +2507,8 @@
       <c r="C144" s="1">
         <v>5.99</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>165</v>
       </c>
@@ -3092,11 +2518,8 @@
       <c r="C145" s="1">
         <v>4.5</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>165</v>
       </c>
@@ -3106,11 +2529,8 @@
       <c r="C146" s="1">
         <v>4.5</v>
       </c>
-      <c r="D146" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>165</v>
       </c>
@@ -3120,11 +2540,8 @@
       <c r="C147" s="1">
         <v>3.99</v>
       </c>
-      <c r="D147" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>165</v>
       </c>
@@ -3134,11 +2551,8 @@
       <c r="C148" s="1">
         <v>6.99</v>
       </c>
-      <c r="D148" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>165</v>
       </c>
@@ -3148,11 +2562,8 @@
       <c r="C149" s="1">
         <v>4.99</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>173</v>
       </c>
@@ -3162,11 +2573,8 @@
       <c r="C150" s="1">
         <v>3</v>
       </c>
-      <c r="D150" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>173</v>
       </c>
@@ -3176,11 +2584,8 @@
       <c r="C151" s="1">
         <v>4.5</v>
       </c>
-      <c r="D151" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>173</v>
       </c>
@@ -3190,11 +2595,8 @@
       <c r="C152" s="1">
         <v>4</v>
       </c>
-      <c r="D152" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>173</v>
       </c>
@@ -3204,11 +2606,8 @@
       <c r="C153" s="1">
         <v>3.5</v>
       </c>
-      <c r="D153" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>173</v>
       </c>
@@ -3218,11 +2617,8 @@
       <c r="C154" s="1">
         <v>4.5</v>
       </c>
-      <c r="D154" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>173</v>
       </c>
@@ -3232,11 +2628,8 @@
       <c r="C155" s="1">
         <v>3.5</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>173</v>
       </c>
@@ -3246,11 +2639,8 @@
       <c r="C156" s="1">
         <v>3.5</v>
       </c>
-      <c r="D156" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>173</v>
       </c>
@@ -3259,9 +2649,6 @@
       </c>
       <c r="C157" s="1">
         <v>3.5</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>